<commit_message>
Versión 1.5 con peso planta, resumen aplicaciones por categoria y categoria por insumo
</commit_message>
<xml_diff>
--- a/relacion_insumos_principales_categorias.xlsx
+++ b/relacion_insumos_principales_categorias.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://agricolaguapa.sharepoint.com/sites/BI/Documentos compartidos/seguimiento_nutricion/preprocesamiento/consultas_postgresql_gcp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://agricolaguapa.sharepoint.com/sites/BI/Documentos compartidos/seguimiento_nutricion/webapp/guapa_seguimiento_nutricion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="67" documentId="11_1888A360A95C1B04BD12A2809B206BB82A698A09" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{049017DA-BA6C-46D9-B3AC-47B09B9DC9A0}"/>
+  <xr:revisionPtr revIDLastSave="69" documentId="11_1888A360A95C1B04BD12A2809B206BB82A698A09" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7AB204C0-AD4D-4DF4-BD98-DA19D71CD334}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3617,21 +3617,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100A33E34522131A74E987C513863CC999E" ma:contentTypeVersion="8" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="f8c4db5e6fb2db0844291ed35b4457df">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cf82246f-0d56-4e35-bddb-fe678e52f926" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a1191df063dea3730b9d6f4cb4be4c39" ns2:_="">
     <xsd:import namespace="cf82246f-0d56-4e35-bddb-fe678e52f926"/>
@@ -3803,24 +3788,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{619AD138-E3EF-4169-A988-A13B38BEBF7C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1777E837-EF34-4231-8417-79037579D9CF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA20AA56-DCCB-43EC-B357-6BD9EBC58FF3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3836,4 +3819,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1777E837-EF34-4231-8417-79037579D9CF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{619AD138-E3EF-4169-A988-A13B38BEBF7C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>